<commit_message>
data formatting standardization for steel (not tested)
</commit_message>
<xml_diff>
--- a/scenarios-examples/not ready/steel_raw/data/fuels.xlsx
+++ b/scenarios-examples/not ready/steel_raw/data/fuels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wajju/GitHub/BlackBlox/scenarios-examples/not ready/steel_raw/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025D0304-7CF0-D643-9E51-CE4D83D8DEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82FD06E-950D-1B4B-BE0D-5896D8559AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="460" windowWidth="16760" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="500" windowWidth="28840" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fuels" sheetId="2" r:id="rId1"/>
@@ -32,82 +32,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="L16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>from https://www.forestresearch.gov.uk/tools-and-resources/biomass-energy-resources/reference-biomass/facts-figures/carbon-emissions-of-different-fuels/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>calculated from Swanson 2010 (HT scenario)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="fuels" type="6" refreshedVersion="6" background="1" saveData="1">
@@ -124,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>meta-notes</t>
   </si>
@@ -150,30 +74,12 @@
     <t>meta-source</t>
   </si>
   <si>
-    <t>Moisture Content</t>
-  </si>
-  <si>
-    <t>t / t wet</t>
-  </si>
-  <si>
     <t>LHV</t>
   </si>
   <si>
     <t>(gj/t dry)</t>
   </si>
   <si>
-    <t>C %</t>
-  </si>
-  <si>
-    <t>H %</t>
-  </si>
-  <si>
-    <t>S %</t>
-  </si>
-  <si>
-    <t>Ash %</t>
-  </si>
-  <si>
     <t>IPCC EFDB</t>
   </si>
   <si>
@@ -189,15 +95,9 @@
     <t>http://www.fao.org/3/a-i6935e.pdf</t>
   </si>
   <si>
-    <t>WEO 2018</t>
-  </si>
-  <si>
     <t>charcoal - IPCC</t>
   </si>
   <si>
-    <t>rice hulls - IPCC</t>
-  </si>
-  <si>
     <t>wood oven dry - IPCC</t>
   </si>
   <si>
@@ -210,45 +110,18 @@
     <t>coal bituminous - IPCC</t>
   </si>
   <si>
-    <t>electricity PROXY - EU 2016</t>
-  </si>
-  <si>
-    <t>electricity PROXY - decarbonized</t>
-  </si>
-  <si>
-    <t>electricity PROXY - CN 2016</t>
-  </si>
-  <si>
-    <t>syngas - ecoinvent</t>
-  </si>
-  <si>
-    <t>syngas - PNNL</t>
-  </si>
-  <si>
     <t>wood chips - dry</t>
   </si>
   <si>
-    <t>charcoal-low upstream</t>
-  </si>
-  <si>
-    <t>charcoal-high upstream</t>
-  </si>
-  <si>
     <t>diesel</t>
   </si>
   <si>
     <t>ecoinvent 2.2</t>
   </si>
   <si>
-    <t>Debt CO2</t>
-  </si>
-  <si>
     <t>coal - CEMCAP</t>
   </si>
   <si>
-    <t>syngas - NREL</t>
-  </si>
-  <si>
     <t>syngas - wood</t>
   </si>
   <si>
@@ -276,43 +149,16 @@
     <t>dry wood chips (EU no swiss) also</t>
   </si>
   <si>
-    <t>dry black liquor</t>
-  </si>
-  <si>
-    <t>%DM</t>
-  </si>
-  <si>
-    <t>HFO - IEAGHG</t>
-  </si>
-  <si>
     <t>recovered steam</t>
   </si>
   <si>
     <t>HFO - IPCC</t>
   </si>
   <si>
-    <t>strong black liquor</t>
-  </si>
-  <si>
-    <t>biosludge (dry)</t>
-  </si>
-  <si>
-    <t>biosludge</t>
-  </si>
-  <si>
-    <t>hog fuel</t>
-  </si>
-  <si>
-    <t>hog fuel (dry)</t>
-  </si>
-  <si>
     <t>CO2__fossil</t>
   </si>
   <si>
     <t>CO2__bio</t>
-  </si>
-  <si>
-    <t>charcoal - inhouse</t>
   </si>
 </sst>
 </file>
@@ -323,7 +169,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -465,27 +311,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -792,7 +617,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -835,26 +660,18 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -888,7 +705,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1212,14 +1028,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1228,15 +1044,10 @@
     <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" customWidth="1"/>
     <col min="4" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" customWidth="1"/>
-    <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1244,43 +1055,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1289,18 +1079,9 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1308,7 +1089,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
@@ -1318,79 +1099,41 @@
         <v>4</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B4"/>
       <c r="C4">
         <v>29.5</v>
       </c>
       <c r="E4">
-        <f>112*C4/1000</f>
         <v>3.3039999999999998</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7">
-        <f>E4*$G$2</f>
-        <v>0.99119999999999986</v>
-      </c>
-      <c r="H4"/>
-      <c r="I4">
-        <v>0.91</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="M4"/>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="4"/>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B5"/>
       <c r="C5">
         <v>26.7</v>
       </c>
       <c r="D5">
-        <f>98.3*C5/1000</f>
         <v>2.6246099999999997</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5">
-        <v>0.67</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-    </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>25.8</v>
@@ -1399,24 +1142,15 @@
         <v>25.8</v>
       </c>
       <c r="D6">
-        <f>96.1*C6/1000</f>
         <v>2.4793799999999999</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6">
-        <v>0.67</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-    </row>
-    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>27.1</v>
@@ -1425,24 +1159,15 @@
         <v>27.1</v>
       </c>
       <c r="D7">
-        <f>I7*(44/12)</f>
         <v>2.5299999999999998</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7">
-        <v>0.69</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>28.2</v>
@@ -1451,19 +1176,15 @@
         <v>28.2</v>
       </c>
       <c r="D8">
-        <f>94.6*C8/1000</f>
         <v>2.6677199999999996</v>
       </c>
-      <c r="I8">
-        <v>0.73</v>
-      </c>
-      <c r="N8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>28.2</v>
@@ -1472,16 +1193,12 @@
         <v>28.2</v>
       </c>
       <c r="D9">
-        <f>107*C9/1000</f>
         <v>3.0174000000000003</v>
       </c>
-      <c r="I9">
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>48</v>
@@ -1490,580 +1207,230 @@
         <v>48</v>
       </c>
       <c r="D10">
-        <f>56.1*C10/1000</f>
         <v>2.6928000000000001</v>
       </c>
-      <c r="I10">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E12">
         <v>0</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="N11" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>21.5</v>
+      </c>
+      <c r="C13">
+        <v>21.5</v>
+      </c>
+      <c r="E13">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4">
-        <v>14.4</v>
-      </c>
-      <c r="E14">
-        <f>100*C14/1000</f>
-        <v>1.44</v>
-      </c>
-      <c r="G14" s="7">
-        <f t="shared" ref="G14:G23" si="0">E14*$G$2</f>
-        <v>0.432</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
       <c r="B15">
-        <v>20</v>
+        <v>45.6</v>
       </c>
       <c r="C15">
-        <v>20</v>
-      </c>
-      <c r="E15">
-        <f>112*C15/1000</f>
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="G15" s="7">
-        <f t="shared" si="0"/>
-        <v>0.67200000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>28.434999999999999</v>
+      </c>
+      <c r="D15">
+        <v>3.1533333333333333</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
       <c r="C16">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
         <v>0</v>
       </c>
-      <c r="G16" s="7">
-        <f t="shared" si="0"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
         <v>0</v>
       </c>
-      <c r="L16">
-        <f>22*C16/1000</f>
-        <v>0.36520000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17">
-        <v>21.5</v>
-      </c>
-      <c r="C17">
-        <v>21.5</v>
-      </c>
-      <c r="E17">
-        <v>1.3</v>
-      </c>
-      <c r="G17" s="7">
-        <f t="shared" si="0"/>
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B18">
-        <v>21.5</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>21.5</v>
-      </c>
-      <c r="E18">
-        <v>1.3</v>
-      </c>
-      <c r="G18" s="7">
-        <f t="shared" si="0"/>
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B19">
-        <f>5.4/1.15</f>
-        <v>4.6956521739130439</v>
-      </c>
-      <c r="C19">
-        <f>5.4/1.15</f>
-        <v>4.6956521739130439</v>
-      </c>
-      <c r="E19">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="G19" s="7">
-        <f t="shared" si="0"/>
-        <v>0.27810000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="E22">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B20">
-        <v>27.662990000000001</v>
-      </c>
-      <c r="C20">
-        <v>27.662990000000001</v>
-      </c>
-      <c r="E20">
-        <v>1.392744</v>
-      </c>
-      <c r="G20" s="7">
-        <f t="shared" si="0"/>
-        <v>0.41782320000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="E23">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="C21">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="G21" s="7">
-        <f t="shared" si="0"/>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="C22">
-        <v>29.5</v>
-      </c>
-      <c r="E22">
-        <f>112*C22/1000</f>
-        <v>3.3039999999999998</v>
-      </c>
-      <c r="G22" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99119999999999986</v>
-      </c>
-      <c r="I22">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23">
-        <v>29.5</v>
-      </c>
-      <c r="E23">
-        <f>112*C23/1000</f>
-        <v>3.3039999999999998</v>
-      </c>
-      <c r="G23" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99119999999999986</v>
-      </c>
-      <c r="I23">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24">
-        <v>45.6</v>
-      </c>
-      <c r="C24">
-        <v>28.434999999999999</v>
-      </c>
-      <c r="D24">
-        <f>I24*(44/12)</f>
-        <v>3.1533333333333333</v>
-      </c>
-      <c r="G24" s="7"/>
-      <c r="I24">
-        <v>0.86</v>
-      </c>
-      <c r="N24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
       <c r="B25">
-        <v>1</v>
+        <v>40.4</v>
       </c>
       <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31">
-        <f t="shared" ref="B31:C32" si="1">B$15</f>
-        <v>20</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="E31">
-        <f>E$15</f>
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="E32">
-        <f>E$15</f>
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33">
-        <v>20.5</v>
-      </c>
-      <c r="C33">
-        <v>20.5</v>
-      </c>
-      <c r="E33">
-        <f>I33*(44/12)</f>
-        <v>1.8296666666666666</v>
-      </c>
-      <c r="I33">
-        <v>0.499</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34">
-        <f>B33*(1-$H34)</f>
-        <v>10.25</v>
-      </c>
-      <c r="C34">
-        <f>C33*(1-$H34)</f>
-        <v>10.25</v>
-      </c>
-      <c r="E34">
-        <f>E33*(1-$H34)</f>
-        <v>0.91483333333333328</v>
-      </c>
-      <c r="H34">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35">
-        <v>13.7</v>
-      </c>
-      <c r="C35">
-        <v>13.7</v>
-      </c>
-      <c r="E35">
-        <f>I35*(44/12)</f>
-        <v>1.1366666666666667</v>
-      </c>
-      <c r="I35">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36">
-        <f>B35*(1-$H36)</f>
-        <v>10.96</v>
-      </c>
-      <c r="C36">
-        <f>C35*(1-$H36)</f>
-        <v>10.96</v>
-      </c>
-      <c r="E36">
-        <f>E35*(1-$H36)</f>
-        <v>0.90933333333333344</v>
-      </c>
-      <c r="F36">
-        <f>H36</f>
-        <v>0.2</v>
-      </c>
-      <c r="H36">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37">
-        <v>20</v>
-      </c>
-      <c r="C37">
-        <v>20</v>
-      </c>
-      <c r="E37">
-        <f>I37*(44/12)</f>
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="F37" s="9"/>
-      <c r="H37" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="I37">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38">
-        <f>B37*(1-$H37)</f>
-        <v>8</v>
-      </c>
-      <c r="C38">
-        <f>C37*(1-$H37)</f>
-        <v>8</v>
-      </c>
-      <c r="E38">
-        <f>E37*(1-$H37)</f>
-        <v>0.73333333333333339</v>
-      </c>
-      <c r="F38" s="10">
-        <f>H37</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39">
-        <v>41</v>
-      </c>
-      <c r="C39">
-        <v>41</v>
-      </c>
-      <c r="D39">
-        <f>D24</f>
-        <v>3.1533333333333333</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41">
         <v>40.4</v>
       </c>
-      <c r="C41">
-        <v>40.4</v>
-      </c>
-      <c r="D41">
-        <f>77.4*C41/1000</f>
+      <c r="D25">
         <v>3.12696</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42">
-        <v>29.5</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42">
-        <f>112*C42/1000</f>
-        <v>3.3039999999999998</v>
-      </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7">
-        <f>E42*$G$2</f>
-        <v>0.99119999999999986</v>
-      </c>
-      <c r="I42">
-        <v>0.91</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>